<commit_message>
Ajout accent police bebas
</commit_message>
<xml_diff>
--- a/Planification/Estimation.xlsx
+++ b/Planification/Estimation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CFCCAD-FD47-40FE-93C5-C214E78A4ED1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D160815F-C9EA-4E14-BE87-EA56E074B193}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -139,6 +139,24 @@
   </si>
   <si>
     <t>Ajout de boutons sur la carte qui affichera une photo de salle qu'on a touché</t>
+  </si>
+  <si>
+    <t>Création de l'app, création du logo, développement de ma vue du main menu</t>
+  </si>
+  <si>
+    <t>Recherche et implémentation du expandableListView avec pager adapter (données hard code pour l'instant)</t>
+  </si>
+  <si>
+    <t>Création du modèle relationnel de ma BD + fin implémentation listView</t>
+  </si>
+  <si>
+    <t>Début de la création de mon modèle SQLITE dans mon app android</t>
+  </si>
+  <si>
+    <t>Fin modèle SQLITE + début création BD avec sqlite data browser</t>
+  </si>
+  <si>
+    <t>J'ai bien enclenché le projet, par contre, je pourrais mettre plus d'heure pour la prochaine itération.</t>
   </si>
 </sst>
 </file>
@@ -282,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,6 +351,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1714,7 +1735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A6:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -1943,8 +1964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,117 +2022,147 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="23">
+        <v>43179</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="15">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="23">
+        <v>43180</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="15">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="23">
+        <v>43181</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="23">
+        <v>43186</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="23">
+        <v>43187</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+      <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+      <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
+      <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+      <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+      <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+      <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
+      <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
@@ -2122,7 +2173,7 @@
       <c r="B37" s="19"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2135,7 +2186,9 @@
       <c r="A40" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
@@ -2144,7 +2197,9 @@
       <c r="A42" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="20"/>
+      <c r="B42" s="20" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="21"/>

</xml_diff>